<commit_message>
Homework 1 and additional files.
</commit_message>
<xml_diff>
--- a/Lectures/S2025/Lectures/W4111-2025S-12-Module-II-NoSQL-Module-IV-1/pivot-tables-example.xlsx
+++ b/Lectures/S2025/Lectures/W4111-2025S-12-Module-II-NoSQL-Module-IV-1/pivot-tables-example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/donald.ferguson/Dropbox/000/000-Columbia-Courses/W4111-Introduction-to-Databases/Lectures/S2025/Lectures/W4111-2025S-12-Module-II-NoSQL-Module-IV-1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3B903E40-7E08-5E4C-9F6C-DDDF11CB73E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A891C02B-30C6-CA41-B8A4-8C7BFF3BAD3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9160" yWindow="3360" windowWidth="34120" windowHeight="19800" tabRatio="796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4180" yWindow="2780" windowWidth="34120" windowHeight="19800" tabRatio="796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Two-dimensional Pivot Table" sheetId="4" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="714" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="53">
   <si>
     <t>Country</t>
   </si>
@@ -2587,7 +2587,7 @@
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable2" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="A3:I48" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <location ref="A3:I33" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
     <pivotField axis="axisCol" showAll="0">
@@ -2617,28 +2617,28 @@
         <item x="3"/>
         <item x="4"/>
         <item x="5"/>
-        <item x="6"/>
+        <item sd="0" x="6"/>
         <item x="7"/>
-        <item x="8"/>
+        <item sd="0" x="8"/>
         <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
+        <item sd="0" x="10"/>
+        <item sd="0" x="11"/>
         <item x="12"/>
         <item x="13"/>
         <item x="14"/>
         <item x="15"/>
-        <item x="16"/>
+        <item sd="0" x="16"/>
         <item x="17"/>
-        <item x="18"/>
+        <item sd="0" x="18"/>
         <item x="19"/>
-        <item x="20"/>
+        <item sd="0" x="20"/>
         <item x="21"/>
-        <item x="22"/>
+        <item sd="0" x="22"/>
         <item x="23"/>
-        <item x="24"/>
+        <item sd="0" x="24"/>
         <item x="25"/>
         <item x="26"/>
-        <item x="27"/>
+        <item sd="0" x="27"/>
         <item x="28"/>
         <item x="29"/>
         <item x="30"/>
@@ -3019,15 +3019,12 @@
     <field x="4"/>
     <field x="5"/>
   </rowFields>
-  <rowItems count="44">
+  <rowItems count="29">
     <i>
       <x v="1"/>
     </i>
     <i r="1">
       <x v="5"/>
-    </i>
-    <i r="2">
-      <x v="6"/>
     </i>
     <i r="1">
       <x v="6"/>
@@ -3038,71 +3035,29 @@
     <i r="1">
       <x v="7"/>
     </i>
-    <i r="2">
-      <x v="6"/>
-    </i>
     <i r="1">
       <x v="9"/>
-    </i>
-    <i r="2">
-      <x v="1"/>
-    </i>
-    <i r="2">
-      <x v="3"/>
     </i>
     <i r="1">
       <x v="10"/>
     </i>
-    <i r="2">
-      <x/>
-    </i>
-    <i r="2">
-      <x v="6"/>
-    </i>
     <i r="1">
       <x v="15"/>
-    </i>
-    <i r="2">
-      <x v="1"/>
-    </i>
-    <i r="2">
-      <x v="2"/>
-    </i>
-    <i r="2">
-      <x v="3"/>
-    </i>
-    <i r="2">
-      <x v="4"/>
     </i>
     <i r="1">
       <x v="17"/>
     </i>
-    <i r="2">
-      <x v="6"/>
-    </i>
     <i r="1">
       <x v="19"/>
-    </i>
-    <i r="2">
-      <x v="3"/>
     </i>
     <i r="1">
       <x v="21"/>
     </i>
-    <i r="2">
-      <x v="1"/>
-    </i>
     <i r="1">
       <x v="23"/>
     </i>
-    <i r="2">
-      <x v="2"/>
-    </i>
     <i r="1">
       <x v="26"/>
-    </i>
-    <i r="2">
-      <x v="5"/>
     </i>
     <i r="1">
       <x v="27"/>
@@ -4074,15 +4029,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I48"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" zoomScale="245" zoomScaleNormal="245" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.1640625" bestFit="1" customWidth="1"/>
@@ -4169,25 +4124,25 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="8" t="s">
-        <v>8</v>
+      <c r="A7" s="7" t="s">
+        <v>29</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6">
-        <v>4270</v>
-      </c>
+      <c r="E7" s="6">
+        <v>8239</v>
+      </c>
+      <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6">
-        <v>4270</v>
+        <v>8239</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="7" t="s">
-        <v>29</v>
+      <c r="A8" s="8" t="s">
+        <v>9</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -4203,171 +4158,171 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="8" t="s">
-        <v>9</v>
+      <c r="A9" s="7" t="s">
+        <v>30</v>
       </c>
       <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
+      <c r="C9" s="6">
+        <v>617</v>
+      </c>
       <c r="D9" s="6"/>
-      <c r="E9" s="6">
-        <v>8239</v>
-      </c>
+      <c r="E9" s="6"/>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6">
-        <v>8239</v>
+        <v>617</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6">
-        <v>617</v>
-      </c>
-      <c r="D10" s="6"/>
+        <v>8384</v>
+      </c>
+      <c r="D10" s="6">
+        <v>2626</v>
+      </c>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6">
-        <v>617</v>
+        <v>11010</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="8" t="s">
-        <v>8</v>
+      <c r="A11" s="7" t="s">
+        <v>32</v>
       </c>
       <c r="B11" s="6"/>
-      <c r="C11" s="6">
-        <v>617</v>
-      </c>
+      <c r="C11" s="6"/>
       <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
+      <c r="E11" s="6">
+        <v>9062</v>
+      </c>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
+      <c r="H11" s="6">
+        <v>3610</v>
+      </c>
       <c r="I11" s="6">
-        <v>617</v>
+        <v>12672</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" s="6"/>
+        <v>33</v>
+      </c>
+      <c r="B12" s="6">
+        <v>9848</v>
+      </c>
       <c r="C12" s="6">
-        <v>8384</v>
-      </c>
-      <c r="D12" s="6">
-        <v>2626</v>
-      </c>
+        <v>15156</v>
+      </c>
+      <c r="D12" s="6"/>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
       <c r="I12" s="6">
-        <v>11010</v>
+        <v>25004</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="8" t="s">
-        <v>10</v>
+      <c r="A13" s="7" t="s">
+        <v>34</v>
       </c>
       <c r="B13" s="6"/>
-      <c r="C13" s="6">
-        <v>8384</v>
-      </c>
+      <c r="C13" s="6"/>
       <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
+      <c r="E13" s="6">
+        <v>7012</v>
+      </c>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
       <c r="I13" s="6">
-        <v>8384</v>
+        <v>7012</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="8" t="s">
-        <v>12</v>
+      <c r="A14" s="7" t="s">
+        <v>35</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
-      <c r="D14" s="6">
-        <v>2626</v>
-      </c>
+      <c r="D14" s="6"/>
       <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
+      <c r="F14" s="6">
+        <v>1903</v>
+      </c>
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
       <c r="I14" s="6">
-        <v>2626</v>
+        <v>1903</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6">
-        <v>9062</v>
+        <v>2824</v>
       </c>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
-      <c r="H15" s="6">
-        <v>3610</v>
-      </c>
+      <c r="H15" s="6"/>
       <c r="I15" s="6">
-        <v>12672</v>
+        <v>2824</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" s="6"/>
+      <c r="A16" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="6">
+        <v>6946</v>
+      </c>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
-      <c r="E16" s="6">
-        <v>9062</v>
-      </c>
+      <c r="E16" s="6"/>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
       <c r="I16" s="6">
-        <v>9062</v>
+        <v>6946</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="8" t="s">
-        <v>8</v>
+      <c r="A17" s="7" t="s">
+        <v>38</v>
       </c>
       <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
+      <c r="C17" s="6">
+        <v>2320</v>
+      </c>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
-      <c r="H17" s="6">
-        <v>3610</v>
-      </c>
+      <c r="H17" s="6"/>
       <c r="I17" s="6">
-        <v>3610</v>
+        <v>2320</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" s="6">
-        <v>9848</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="B18" s="6"/>
       <c r="C18" s="6">
-        <v>15156</v>
+        <v>2116</v>
       </c>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
@@ -4375,636 +4330,381 @@
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
       <c r="I18" s="6">
-        <v>25004</v>
+        <v>2116</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B19" s="6">
-        <v>7431</v>
-      </c>
-      <c r="C19" s="6"/>
+        <v>8</v>
+      </c>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6">
+        <v>2116</v>
+      </c>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
       <c r="I19" s="6">
-        <v>7431</v>
+        <v>2116</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20" s="6">
-        <v>2417</v>
-      </c>
-      <c r="C20" s="6"/>
+      <c r="A20" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6">
+        <v>1135</v>
+      </c>
       <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
+      <c r="E20" s="6">
+        <v>3595</v>
+      </c>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
       <c r="I20" s="6">
-        <v>2417</v>
+        <v>4730</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B21" s="6"/>
       <c r="C21" s="6">
-        <v>8250</v>
+        <v>1135</v>
       </c>
       <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
+      <c r="E21" s="6">
+        <v>3595</v>
+      </c>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
       <c r="H21" s="6"/>
       <c r="I21" s="6">
-        <v>8250</v>
+        <v>4730</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22" s="6"/>
+      <c r="A22" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="6">
+        <v>19715</v>
+      </c>
       <c r="C22" s="6">
-        <v>6906</v>
-      </c>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
+        <v>9228</v>
+      </c>
+      <c r="D22" s="6">
+        <v>15823</v>
+      </c>
+      <c r="E22" s="6">
+        <v>1557</v>
+      </c>
+      <c r="F22" s="6">
+        <v>5154</v>
+      </c>
+      <c r="G22" s="6">
+        <v>9029</v>
+      </c>
+      <c r="H22" s="6">
+        <v>2256</v>
+      </c>
       <c r="I22" s="6">
-        <v>6906</v>
+        <v>62762</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
+      <c r="A23" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" s="6">
+        <v>25702</v>
+      </c>
+      <c r="C23" s="6">
+        <v>26224</v>
+      </c>
+      <c r="D23" s="6">
+        <v>6045</v>
+      </c>
       <c r="E23" s="6">
-        <v>7012</v>
-      </c>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
+        <v>5341</v>
+      </c>
+      <c r="F23" s="6">
+        <v>21722</v>
+      </c>
+      <c r="G23" s="6">
+        <v>3663</v>
+      </c>
+      <c r="H23" s="6">
+        <v>15869</v>
+      </c>
       <c r="I23" s="6">
-        <v>7012</v>
+        <v>104566</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
+      <c r="A24" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" s="6">
+        <v>14586</v>
+      </c>
+      <c r="C24" s="6">
+        <v>16001</v>
+      </c>
       <c r="D24" s="6"/>
       <c r="E24" s="6">
-        <v>7012</v>
-      </c>
-      <c r="F24" s="6"/>
+        <v>9508</v>
+      </c>
+      <c r="F24" s="6">
+        <v>8266</v>
+      </c>
       <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
+      <c r="H24" s="6">
+        <v>1113</v>
+      </c>
       <c r="I24" s="6">
-        <v>7012</v>
+        <v>49474</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
+      <c r="A25" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" s="6">
+        <v>22557</v>
+      </c>
+      <c r="C25" s="6">
+        <v>69521</v>
+      </c>
+      <c r="D25" s="6">
+        <v>8096</v>
+      </c>
+      <c r="E25" s="6">
+        <v>17104</v>
+      </c>
       <c r="F25" s="6">
-        <v>1903</v>
-      </c>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
+        <v>28887</v>
+      </c>
+      <c r="G25" s="6">
+        <v>33384</v>
+      </c>
+      <c r="H25" s="6">
+        <v>23790</v>
+      </c>
       <c r="I25" s="6">
-        <v>1903</v>
+        <v>203339</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
+      <c r="A26" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B26" s="6">
+        <v>6126</v>
+      </c>
+      <c r="C26" s="6">
+        <v>15208</v>
+      </c>
       <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6">
-        <v>1903</v>
-      </c>
+      <c r="E26" s="6">
+        <v>25752</v>
+      </c>
+      <c r="F26" s="6"/>
       <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
+      <c r="H26" s="6">
+        <v>4514</v>
+      </c>
       <c r="I26" s="6">
-        <v>1903</v>
+        <v>51600</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
+      <c r="A27" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B27" s="6">
+        <v>2034</v>
+      </c>
+      <c r="C27" s="6">
+        <v>31336</v>
+      </c>
+      <c r="D27" s="6">
+        <v>8416</v>
+      </c>
       <c r="E27" s="6">
-        <v>2824</v>
-      </c>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
+        <v>13170</v>
+      </c>
+      <c r="F27" s="6">
+        <v>5751</v>
+      </c>
+      <c r="G27" s="6">
+        <v>5480</v>
+      </c>
+      <c r="H27" s="6">
+        <v>14548</v>
+      </c>
       <c r="I27" s="6">
-        <v>2824</v>
+        <v>80735</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
+      <c r="A28" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B28" s="6">
+        <v>22611</v>
+      </c>
+      <c r="C28" s="6">
+        <v>9980</v>
+      </c>
+      <c r="D28" s="6">
+        <v>5761</v>
+      </c>
       <c r="E28" s="6">
-        <v>2824</v>
-      </c>
-      <c r="F28" s="6"/>
+        <v>20386</v>
+      </c>
+      <c r="F28" s="6">
+        <v>9397</v>
+      </c>
       <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
+      <c r="H28" s="6">
+        <v>859</v>
+      </c>
       <c r="I28" s="6">
-        <v>2824</v>
+        <v>68994</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" s="7" t="s">
-        <v>37</v>
+      <c r="A29" s="5" t="s">
+        <v>49</v>
       </c>
       <c r="B29" s="6">
-        <v>6946</v>
-      </c>
-      <c r="C29" s="6"/>
+        <v>8489</v>
+      </c>
+      <c r="C29" s="6">
+        <v>51835</v>
+      </c>
       <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
+      <c r="E29" s="6">
+        <v>18605</v>
+      </c>
+      <c r="F29" s="6">
+        <v>7933</v>
+      </c>
+      <c r="G29" s="6">
+        <v>5523</v>
+      </c>
+      <c r="H29" s="6">
+        <v>10048</v>
+      </c>
       <c r="I29" s="6">
-        <v>6946</v>
+        <v>102433</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30" s="8" t="s">
-        <v>20</v>
+      <c r="A30" s="5" t="s">
+        <v>50</v>
       </c>
       <c r="B30" s="6">
-        <v>6946</v>
-      </c>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
+        <v>15331</v>
+      </c>
+      <c r="C30" s="6">
+        <v>22320</v>
+      </c>
+      <c r="D30" s="6">
+        <v>5015</v>
+      </c>
       <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
+      <c r="F30" s="6">
+        <v>9949</v>
+      </c>
       <c r="G30" s="6"/>
       <c r="H30" s="6"/>
       <c r="I30" s="6">
-        <v>6946</v>
+        <v>52615</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A31" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="B31" s="6"/>
+      <c r="A31" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B31" s="6">
+        <v>11978</v>
+      </c>
       <c r="C31" s="6">
-        <v>2320</v>
+        <v>29530</v>
       </c>
       <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
+      <c r="E31" s="6">
+        <v>284</v>
+      </c>
+      <c r="F31" s="6">
+        <v>7857</v>
+      </c>
       <c r="G31" s="6"/>
-      <c r="H31" s="6"/>
+      <c r="H31" s="6">
+        <v>24091</v>
+      </c>
       <c r="I31" s="6">
-        <v>2320</v>
+        <v>73740</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A32" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B32" s="6"/>
+      <c r="A32" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B32" s="6">
+        <v>25334</v>
+      </c>
       <c r="C32" s="6">
-        <v>2320</v>
-      </c>
-      <c r="D32" s="6"/>
+        <v>29384</v>
+      </c>
+      <c r="D32" s="6">
+        <v>5499</v>
+      </c>
       <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
+      <c r="F32" s="6">
+        <v>25856</v>
+      </c>
       <c r="G32" s="6"/>
-      <c r="H32" s="6"/>
+      <c r="H32" s="6">
+        <v>3740</v>
+      </c>
       <c r="I32" s="6">
-        <v>2320</v>
+        <v>89813</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A33" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B33" s="6"/>
+      <c r="A33" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B33" s="6">
+        <v>191257</v>
+      </c>
       <c r="C33" s="6">
-        <v>2116</v>
-      </c>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="6"/>
-      <c r="G33" s="6"/>
-      <c r="H33" s="6"/>
+        <v>340295</v>
+      </c>
+      <c r="D33" s="6">
+        <v>57281</v>
+      </c>
+      <c r="E33" s="6">
+        <v>142439</v>
+      </c>
+      <c r="F33" s="6">
+        <v>136945</v>
+      </c>
+      <c r="G33" s="6">
+        <v>57079</v>
+      </c>
+      <c r="H33" s="6">
+        <v>104438</v>
+      </c>
       <c r="I33" s="6">
-        <v>2116</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A34" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B34" s="6"/>
-      <c r="C34" s="6">
-        <v>2116</v>
-      </c>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
-      <c r="G34" s="6"/>
-      <c r="H34" s="6"/>
-      <c r="I34" s="6">
-        <v>2116</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A35" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="B35" s="6"/>
-      <c r="C35" s="6">
-        <v>1135</v>
-      </c>
-      <c r="D35" s="6"/>
-      <c r="E35" s="6">
-        <v>3595</v>
-      </c>
-      <c r="F35" s="6"/>
-      <c r="G35" s="6"/>
-      <c r="H35" s="6"/>
-      <c r="I35" s="6">
-        <v>4730</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A36" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B36" s="6"/>
-      <c r="C36" s="6">
-        <v>1135</v>
-      </c>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6">
-        <v>3595</v>
-      </c>
-      <c r="F36" s="6"/>
-      <c r="G36" s="6"/>
-      <c r="H36" s="6"/>
-      <c r="I36" s="6">
-        <v>4730</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A37" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B37" s="6">
-        <v>19715</v>
-      </c>
-      <c r="C37" s="6">
-        <v>9228</v>
-      </c>
-      <c r="D37" s="6">
-        <v>15823</v>
-      </c>
-      <c r="E37" s="6">
-        <v>1557</v>
-      </c>
-      <c r="F37" s="6">
-        <v>5154</v>
-      </c>
-      <c r="G37" s="6">
-        <v>9029</v>
-      </c>
-      <c r="H37" s="6">
-        <v>2256</v>
-      </c>
-      <c r="I37" s="6">
-        <v>62762</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A38" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B38" s="6">
-        <v>25702</v>
-      </c>
-      <c r="C38" s="6">
-        <v>26224</v>
-      </c>
-      <c r="D38" s="6">
-        <v>6045</v>
-      </c>
-      <c r="E38" s="6">
-        <v>5341</v>
-      </c>
-      <c r="F38" s="6">
-        <v>21722</v>
-      </c>
-      <c r="G38" s="6">
-        <v>3663</v>
-      </c>
-      <c r="H38" s="6">
-        <v>15869</v>
-      </c>
-      <c r="I38" s="6">
-        <v>104566</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A39" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B39" s="6">
-        <v>14586</v>
-      </c>
-      <c r="C39" s="6">
-        <v>16001</v>
-      </c>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6">
-        <v>9508</v>
-      </c>
-      <c r="F39" s="6">
-        <v>8266</v>
-      </c>
-      <c r="G39" s="6"/>
-      <c r="H39" s="6">
-        <v>1113</v>
-      </c>
-      <c r="I39" s="6">
-        <v>49474</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A40" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B40" s="6">
-        <v>22557</v>
-      </c>
-      <c r="C40" s="6">
-        <v>69521</v>
-      </c>
-      <c r="D40" s="6">
-        <v>8096</v>
-      </c>
-      <c r="E40" s="6">
-        <v>17104</v>
-      </c>
-      <c r="F40" s="6">
-        <v>28887</v>
-      </c>
-      <c r="G40" s="6">
-        <v>33384</v>
-      </c>
-      <c r="H40" s="6">
-        <v>23790</v>
-      </c>
-      <c r="I40" s="6">
-        <v>203339</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A41" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B41" s="6">
-        <v>6126</v>
-      </c>
-      <c r="C41" s="6">
-        <v>15208</v>
-      </c>
-      <c r="D41" s="6"/>
-      <c r="E41" s="6">
-        <v>25752</v>
-      </c>
-      <c r="F41" s="6"/>
-      <c r="G41" s="6"/>
-      <c r="H41" s="6">
-        <v>4514</v>
-      </c>
-      <c r="I41" s="6">
-        <v>51600</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A42" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B42" s="6">
-        <v>2034</v>
-      </c>
-      <c r="C42" s="6">
-        <v>31336</v>
-      </c>
-      <c r="D42" s="6">
-        <v>8416</v>
-      </c>
-      <c r="E42" s="6">
-        <v>13170</v>
-      </c>
-      <c r="F42" s="6">
-        <v>5751</v>
-      </c>
-      <c r="G42" s="6">
-        <v>5480</v>
-      </c>
-      <c r="H42" s="6">
-        <v>14548</v>
-      </c>
-      <c r="I42" s="6">
-        <v>80735</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A43" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B43" s="6">
-        <v>22611</v>
-      </c>
-      <c r="C43" s="6">
-        <v>9980</v>
-      </c>
-      <c r="D43" s="6">
-        <v>5761</v>
-      </c>
-      <c r="E43" s="6">
-        <v>20386</v>
-      </c>
-      <c r="F43" s="6">
-        <v>9397</v>
-      </c>
-      <c r="G43" s="6"/>
-      <c r="H43" s="6">
-        <v>859</v>
-      </c>
-      <c r="I43" s="6">
-        <v>68994</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A44" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B44" s="6">
-        <v>8489</v>
-      </c>
-      <c r="C44" s="6">
-        <v>51835</v>
-      </c>
-      <c r="D44" s="6"/>
-      <c r="E44" s="6">
-        <v>18605</v>
-      </c>
-      <c r="F44" s="6">
-        <v>7933</v>
-      </c>
-      <c r="G44" s="6">
-        <v>5523</v>
-      </c>
-      <c r="H44" s="6">
-        <v>10048</v>
-      </c>
-      <c r="I44" s="6">
-        <v>102433</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A45" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B45" s="6">
-        <v>15331</v>
-      </c>
-      <c r="C45" s="6">
-        <v>22320</v>
-      </c>
-      <c r="D45" s="6">
-        <v>5015</v>
-      </c>
-      <c r="E45" s="6"/>
-      <c r="F45" s="6">
-        <v>9949</v>
-      </c>
-      <c r="G45" s="6"/>
-      <c r="H45" s="6"/>
-      <c r="I45" s="6">
-        <v>52615</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A46" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B46" s="6">
-        <v>11978</v>
-      </c>
-      <c r="C46" s="6">
-        <v>29530</v>
-      </c>
-      <c r="D46" s="6"/>
-      <c r="E46" s="6">
-        <v>284</v>
-      </c>
-      <c r="F46" s="6">
-        <v>7857</v>
-      </c>
-      <c r="G46" s="6"/>
-      <c r="H46" s="6">
-        <v>24091</v>
-      </c>
-      <c r="I46" s="6">
-        <v>73740</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A47" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B47" s="6">
-        <v>25334</v>
-      </c>
-      <c r="C47" s="6">
-        <v>29384</v>
-      </c>
-      <c r="D47" s="6">
-        <v>5499</v>
-      </c>
-      <c r="E47" s="6"/>
-      <c r="F47" s="6">
-        <v>25856</v>
-      </c>
-      <c r="G47" s="6"/>
-      <c r="H47" s="6">
-        <v>3740</v>
-      </c>
-      <c r="I47" s="6">
-        <v>89813</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A48" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B48" s="6">
-        <v>191257</v>
-      </c>
-      <c r="C48" s="6">
-        <v>340295</v>
-      </c>
-      <c r="D48" s="6">
-        <v>57281</v>
-      </c>
-      <c r="E48" s="6">
-        <v>142439</v>
-      </c>
-      <c r="F48" s="6">
-        <v>136945</v>
-      </c>
-      <c r="G48" s="6">
-        <v>57079</v>
-      </c>
-      <c r="H48" s="6">
-        <v>104438</v>
-      </c>
-      <c r="I48" s="6">
         <v>1029734</v>
       </c>
     </row>

</xml_diff>